<commit_message>
Add number of quotes analysis
</commit_message>
<xml_diff>
--- a/data/Fakespeak-ENG/Analysis_output/news_and_blog/Fakespeak_news_and_blog_quotes.xlsx
+++ b/data/Fakespeak-ENG/Analysis_output/news_and_blog/Fakespeak_news_and_blog_quotes.xlsx
@@ -20,13 +20,14 @@
     <sheet name="2024" sheetId="11" r:id="rId11"/>
     <sheet name="2024_proportion" sheetId="12" r:id="rId12"/>
     <sheet name="Proportion Summary" sheetId="13" r:id="rId13"/>
+    <sheet name="Num Quotes Proportions" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7594" uniqueCount="3978">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7596" uniqueCount="3979">
   <si>
     <t>ID</t>
   </si>
@@ -12601,6 +12602,9 @@
   </si>
   <si>
     <t>year</t>
+  </si>
+  <si>
+    <t>proportion_num_quotes_to_num_articles</t>
   </si>
 </sst>
 </file>
@@ -17784,6 +17788,75 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>3977</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3978</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>2019</v>
+      </c>
+      <c r="B2">
+        <v>4.210526315789473</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2020</v>
+      </c>
+      <c r="B3">
+        <v>5.973451327433628</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>2021</v>
+      </c>
+      <c r="B4">
+        <v>6.605263157894737</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>2022</v>
+      </c>
+      <c r="B5">
+        <v>7.108108108108108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>2023</v>
+      </c>
+      <c r="B6">
+        <v>11.06060606060606</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>2024</v>
+      </c>
+      <c r="B7">
+        <v>9.888888888888889</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B18"/>

</xml_diff>